<commit_message>
remove two columns with only reference and assigned by values
</commit_message>
<xml_diff>
--- a/curator-annotations/Phenotype_Annotations/Phenotype_annotation_SEP_21_2021.xlsx
+++ b/curator-annotations/Phenotype_Annotations/Phenotype_annotation_SEP_21_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjd727/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sba964/Projects/migration-data/curator-annotations/Phenotype_Annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CFD72F-7AA8-D741-87DD-7BED8DADA1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8100F50-7A48-1943-BCA4-888D44F05C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="980" windowWidth="34940" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="600" windowWidth="25400" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
   <si>
     <t>Strain ID</t>
   </si>
@@ -236,16 +236,16 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1409,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="E11" zoomScale="177" workbookViewId="0">
+      <selection activeCell="E15" sqref="A15:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.1640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1796,22 +1796,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>